<commit_message>
TEX:fix pe block diagram.
</commit_message>
<xml_diff>
--- a/DOC/Power.xlsx
+++ b/DOC/Power.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="320" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="PE" sheetId="2" r:id="rId1"/>
@@ -17,15 +17,12 @@
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Internal</t>
   </si>
@@ -175,15 +172,67 @@
   </si>
   <si>
     <t>FC-1000</t>
+  </si>
+  <si>
+    <t>nw</t>
+  </si>
+  <si>
+    <t>mw</t>
+  </si>
+  <si>
+    <t>from ptpx</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>memory</t>
+  </si>
+  <si>
+    <t>Memory represents</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 Internal         Switching           Leakage            Total</t>
+  </si>
+  <si>
+    <t>Power Group      Power            Power               Power              Power   (   %    )  Attrs</t>
+  </si>
+  <si>
+    <t>--------------------------------------------------------------------------------------------------</t>
+  </si>
+  <si>
+    <t>io_pad             0.0000            0.0000            0.0000            0.0000  (   0.00%)</t>
+  </si>
+  <si>
+    <t>memory            42.0345            0.2705        5.6409e+04           42.3614  (  23.03%)</t>
+  </si>
+  <si>
+    <t>black_box          0.0000            0.0000            0.0000            0.0000  (   0.00%)</t>
+  </si>
+  <si>
+    <t>clock_network      1.4283            1.1332          763.9230            2.5622  (   1.39%)</t>
+  </si>
+  <si>
+    <t>register         136.3892            1.0543        2.3841e+04          137.4689  (  74.75%)</t>
+  </si>
+  <si>
+    <t>sequential         0.0000            0.0000            0.0000            0.0000  (   0.00%)</t>
+  </si>
+  <si>
+    <t>combinational      0.5831            0.9131        2.1908e+04            1.5180  (   0.83%)</t>
+  </si>
+  <si>
+    <t>Total            180.4350 mW         3.3711 mW     1.0292e+05 nW       183.9105 mW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0.000E+00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -235,7 +284,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="99">
+  <cellStyleXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -335,8 +384,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -372,8 +429,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="99">
+  <cellStyles count="107">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -423,6 +498,10 @@
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -472,19 +551,13 @@
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -507,11 +580,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -837,10 +905,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:M23"/>
+  <dimension ref="C6:Q29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:H7"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -852,50 +920,71 @@
     <col min="13" max="13" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:12">
+    <row r="6" spans="3:17">
+      <c r="E6" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F6" s="2">
+        <f>1/F8</f>
+        <v>0.1973094170403587</v>
+      </c>
       <c r="G6" s="2">
-        <f>1.4062/1.1415</f>
-        <v>1.2318878668418747</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12">
+        <f>1/G8</f>
+        <v>0.82352941176470595</v>
+      </c>
+      <c r="H6" s="2">
+        <f>1/H8</f>
+        <v>2425.742574257426</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17">
       <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="2">
-        <f>1/F8</f>
-        <v>0.19752135763014136</v>
-      </c>
-      <c r="G7" s="2">
-        <f>1/G8</f>
-        <v>0.81659167247607567</v>
-      </c>
-      <c r="H7" s="2">
-        <f>1/H8</f>
-        <v>243.39205967512393</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F7" s="1">
+        <f>MIN(L12/O12,F8)</f>
+        <v>5.0681818181818192</v>
+      </c>
+      <c r="G7" s="2"/>
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="3:12">
+    <row r="8" spans="3:17">
+      <c r="E8" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F8" s="2">
-        <f>67.3998/13.3129</f>
-        <v>5.0627436546507516</v>
+        <f>L11/O11</f>
+        <v>5.0681818181818192</v>
       </c>
       <c r="G8" s="2">
-        <f>1.5779/1.2885</f>
-        <v>1.2246022506790843</v>
-      </c>
-      <c r="H8" s="2">
-        <f>20.377/4959.6</f>
-        <v>4.1085974675377042E-3</v>
+        <f>M11/P11</f>
+        <v>1.2142857142857142</v>
+      </c>
+      <c r="H8" s="5">
+        <f>N11/Q11</f>
+        <v>4.1224489795918366E-4</v>
       </c>
       <c r="J8" s="1">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="3:12">
+    <row r="9" spans="3:17">
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17">
       <c r="F10" s="1" t="s">
         <v>0</v>
       </c>
@@ -908,8 +997,26 @@
       <c r="I10" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="3:12">
+      <c r="L10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="P10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17">
       <c r="E11" s="4" t="s">
         <v>3</v>
       </c>
@@ -930,8 +1037,29 @@
         <v>0.17096130000000001</v>
       </c>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="3:12">
+      <c r="K11" t="s">
+        <v>53</v>
+      </c>
+      <c r="L11">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1.53</v>
+      </c>
+      <c r="N11">
+        <v>2.02</v>
+      </c>
+      <c r="O11">
+        <v>13.2</v>
+      </c>
+      <c r="P11">
+        <v>1.26</v>
+      </c>
+      <c r="Q11">
+        <v>4900</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17">
       <c r="C12" s="4">
         <v>100</v>
       </c>
@@ -939,24 +1067,33 @@
         <v>5</v>
       </c>
       <c r="F12" s="3">
-        <f>F11/F$8</f>
-        <v>2.7652990068219793E-2</v>
+        <f>N22</f>
+        <v>2.7623318385650221E-2</v>
       </c>
       <c r="G12" s="3">
         <f>G11/G$8</f>
-        <v>2.5232682679510739E-2</v>
+        <v>2.5447058823529413E-2</v>
       </c>
       <c r="H12" s="5">
         <f>H$11/H$8</f>
-        <v>1.4919933258085098E-2</v>
+        <v>0.14869801980198019</v>
       </c>
       <c r="I12" s="3">
         <f>SUM(F12:H12)</f>
-        <v>6.780560600581563E-2</v>
+        <v>0.20176839701115984</v>
       </c>
       <c r="J12" s="3"/>
-    </row>
-    <row r="13" spans="3:12" s="6" customFormat="1">
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12">
+        <v>2.36</v>
+      </c>
+      <c r="O12">
+        <v>4.3799999999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" s="6" customFormat="1">
       <c r="C13" s="4">
         <v>1000</v>
       </c>
@@ -966,28 +1103,28 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ref="F13:G16" si="0">F$12*$C13/$C$12</f>
-        <v>0.27652990068219796</v>
+        <v>0.2762331838565022</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="0"/>
-        <v>0.25232682679510737</v>
+        <v>0.25447058823529412</v>
       </c>
       <c r="H13" s="5">
         <f>H$11/H$8</f>
-        <v>1.4919933258085098E-2</v>
+        <v>0.14869801980198019</v>
       </c>
       <c r="I13" s="3">
         <f>SUM(F13:H13)</f>
-        <v>0.54377666073539033</v>
+        <v>0.67940179189377647</v>
       </c>
       <c r="J13" s="3">
         <f>I13*$J$8</f>
-        <v>34.801706287064981</v>
+        <v>43.481714681201694</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
     </row>
-    <row r="14" spans="3:12" s="6" customFormat="1">
+    <row r="14" spans="3:17" s="6" customFormat="1">
       <c r="C14" s="4">
         <v>700</v>
       </c>
@@ -997,28 +1134,31 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
-        <v>0.19357093047753857</v>
+        <v>0.19336322869955155</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="0"/>
-        <v>0.17662877875657518</v>
+        <v>0.17812941176470587</v>
       </c>
       <c r="H14" s="5">
         <f>H$11/H$8</f>
-        <v>1.4919933258085098E-2</v>
+        <v>0.14869801980198019</v>
       </c>
       <c r="I14" s="3">
         <f>SUM(F14:H14)</f>
-        <v>0.38511964249219882</v>
+        <v>0.52019066026623761</v>
       </c>
       <c r="J14" s="3">
         <f>I14*$J$8</f>
-        <v>24.647657119500725</v>
+        <v>33.292202257039207</v>
       </c>
       <c r="K14"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="3:12" s="6" customFormat="1">
+      <c r="L14">
+        <f>L11/O11</f>
+        <v>5.0681818181818192</v>
+      </c>
+    </row>
+    <row r="15" spans="3:17" s="6" customFormat="1">
       <c r="C15" s="4">
         <v>600</v>
       </c>
@@ -1028,28 +1168,28 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
-        <v>0.16591794040931876</v>
+        <v>0.16573991031390134</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="0"/>
-        <v>0.15139609607706445</v>
+        <v>0.15268235294117649</v>
       </c>
       <c r="H15" s="5">
         <f>H$11/H$8</f>
-        <v>1.4919933258085098E-2</v>
+        <v>0.14869801980198019</v>
       </c>
       <c r="I15" s="3">
         <f>SUM(F15:H15)</f>
-        <v>0.33223396974446834</v>
+        <v>0.46712028305705799</v>
       </c>
       <c r="J15" s="3">
         <f>I15*$J$8</f>
-        <v>21.262974063645974</v>
+        <v>29.895698115651712</v>
       </c>
       <c r="K15"/>
       <c r="L15"/>
     </row>
-    <row r="16" spans="3:12" s="6" customFormat="1">
+    <row r="16" spans="3:17" s="6" customFormat="1">
       <c r="C16" s="4">
         <v>500</v>
       </c>
@@ -1059,28 +1199,28 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
-        <v>0.13826495034109898</v>
+        <v>0.1381165919282511</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="0"/>
-        <v>0.12616341339755369</v>
+        <v>0.12723529411764706</v>
       </c>
       <c r="H16" s="5">
         <f>H$11/H$8</f>
-        <v>1.4919933258085098E-2</v>
+        <v>0.14869801980198019</v>
       </c>
       <c r="I16" s="3">
         <f>SUM(F16:H16)</f>
-        <v>0.27934829699673774</v>
+        <v>0.41404990584787837</v>
       </c>
       <c r="J16" s="3">
         <f>I16*$J$8</f>
-        <v>17.878291007791216</v>
+        <v>26.499193974264216</v>
       </c>
       <c r="K16"/>
       <c r="L16"/>
     </row>
-    <row r="17" spans="3:13" s="6" customFormat="1">
+    <row r="17" spans="3:17" s="6" customFormat="1">
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
@@ -1092,13 +1232,32 @@
       <c r="K17"/>
       <c r="L17"/>
     </row>
-    <row r="19" spans="3:13">
+    <row r="18" spans="3:17">
+      <c r="L18" t="s">
+        <v>55</v>
+      </c>
+      <c r="O18" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+    </row>
+    <row r="19" spans="3:17">
       <c r="E19" s="4" t="s">
         <v>32</v>
       </c>
+      <c r="L19" s="17">
+        <f>42.3614/183.9105</f>
+        <v>0.23033703894013666</v>
+      </c>
       <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="3:13">
+      <c r="O19" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="P19" s="19"/>
+      <c r="Q19" s="19"/>
+    </row>
+    <row r="20" spans="3:17">
       <c r="E20" s="4" t="s">
         <v>14</v>
       </c>
@@ -1115,8 +1274,13 @@
         <f>SUM(F20:H20)</f>
         <v>4.1831399999999998E-2</v>
       </c>
-    </row>
-    <row r="21" spans="3:13">
+      <c r="O20" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+    </row>
+    <row r="21" spans="3:17">
       <c r="E21" s="4" t="s">
         <v>2</v>
       </c>
@@ -1136,16 +1300,83 @@
         <f>SUM(F21:H21)</f>
         <v>4.1831399999999998E-2</v>
       </c>
-    </row>
-    <row r="22" spans="3:13">
+      <c r="L21" s="7">
+        <f>F11*(1-L19)</f>
+        <v>0.10775281454838087</v>
+      </c>
+      <c r="M21" s="18">
+        <f>F11*L19</f>
+        <v>3.2247185451619136E-2</v>
+      </c>
+      <c r="O21" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="P21" s="19"/>
+      <c r="Q21" s="19"/>
+    </row>
+    <row r="22" spans="3:17">
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="3:13">
+      <c r="L22">
+        <f>L21/F8</f>
+        <v>2.1260645022998913E-2</v>
+      </c>
+      <c r="M22" s="6">
+        <f>M21/F7</f>
+        <v>6.3626733626513075E-3</v>
+      </c>
+      <c r="N22" s="9">
+        <f>L22+M22</f>
+        <v>2.7623318385650221E-2</v>
+      </c>
+      <c r="O22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="19"/>
+    </row>
+    <row r="23" spans="3:17">
       <c r="H23" s="5"/>
+      <c r="O23" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+    </row>
+    <row r="24" spans="3:17">
+      <c r="O24" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+    </row>
+    <row r="25" spans="3:17">
+      <c r="O25" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17">
+      <c r="O26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17">
+      <c r="O27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17">
+      <c r="O28" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17">
+      <c r="O29" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F7:H7">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="F6:H6">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1161,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C6:M23"/>
+  <dimension ref="C6:O23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:H8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1184,14 +1415,14 @@
     </row>
     <row r="7" spans="3:10">
       <c r="F7" s="2">
-        <f>1/F8</f>
-        <v>0.19752135763014136</v>
+        <f>MIN(6,PE!F7)</f>
+        <v>5.0681818181818192</v>
       </c>
       <c r="G7" s="2">
         <f>1/G8</f>
         <v>0.81659167247607567</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
         <f>1/H8</f>
         <v>243.39205967512393</v>
       </c>
@@ -1211,7 +1442,7 @@
         <f>1.5779/1.2885</f>
         <v>1.2246022506790843</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="5">
         <f>20.377/4959.6</f>
         <v>4.1085974675377042E-3</v>
       </c>
@@ -1223,6 +1454,9 @@
       <c r="D9" s="4" t="s">
         <v>9</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="10" spans="3:10">
       <c r="F10" s="1" t="s">
@@ -1248,7 +1482,7 @@
       <c r="G11" s="3">
         <v>0.123</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="15">
         <v>9.2E-5</v>
       </c>
       <c r="I11" s="3">
@@ -1264,20 +1498,20 @@
         <v>5</v>
       </c>
       <c r="F12" s="3">
-        <f>F11/F$8</f>
-        <v>2.804803278348007E-2</v>
+        <f>N22</f>
+        <v>2.8041011488457397E-2</v>
       </c>
       <c r="G12" s="3">
         <f>G11/G$8</f>
         <v>0.10044077571455731</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="15">
         <f>H$11/H$8</f>
         <v>2.2392069490111403E-2</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
-        <v>0.15088087798814878</v>
+        <v>0.15087385669312611</v>
       </c>
     </row>
     <row r="13" spans="3:10">
@@ -1289,23 +1523,23 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ref="F13:G16" si="1">F$12*$C13/$C$12</f>
-        <v>0.2804803278348007</v>
+        <v>0.28041011488457396</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" si="1"/>
         <v>1.0044077571455732</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="15">
         <f>H$11/H$8</f>
         <v>2.2392069490111403E-2</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>1.3072801544704853</v>
+        <v>1.3072099415202585</v>
       </c>
       <c r="J13" s="3">
         <f>I13*$J$8</f>
-        <v>83.665929886111059</v>
+        <v>83.661436257296543</v>
       </c>
     </row>
     <row r="14" spans="3:10">
@@ -1317,23 +1551,23 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>0.1963362294843605</v>
+        <v>0.19628708041920176</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
         <v>0.70308543000190116</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="15">
         <f>H$11/H$8</f>
         <v>2.2392069490111403E-2</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>0.92181372897637304</v>
+        <v>0.9217645799112143</v>
       </c>
       <c r="J14" s="3">
         <f>I14*$J$8</f>
-        <v>58.996078654487874</v>
+        <v>58.992933114317715</v>
       </c>
     </row>
     <row r="15" spans="3:10">
@@ -1345,23 +1579,23 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" si="1"/>
-        <v>0.16828819670088041</v>
+        <v>0.1682460689307444</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" si="1"/>
         <v>0.60264465428734393</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="15">
         <f>H$11/H$8</f>
         <v>2.2392069490111403E-2</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>0.79332492047833569</v>
+        <v>0.79328279270819979</v>
       </c>
       <c r="J15" s="3">
         <f>I15*$J$8</f>
-        <v>50.772794910613484</v>
+        <v>50.770098733324787</v>
       </c>
     </row>
     <row r="16" spans="3:10">
@@ -1373,50 +1607,88 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" si="1"/>
-        <v>0.14024016391740035</v>
+        <v>0.14020505744228698</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" si="1"/>
         <v>0.50220387857278659</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="15">
         <f>H$11/H$8</f>
         <v>2.2392069490111403E-2</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
-        <v>0.66483611198029835</v>
+        <v>0.66480100550518495</v>
       </c>
       <c r="J16" s="3">
         <f>I16*$J$8</f>
-        <v>42.549511166739094</v>
-      </c>
-    </row>
-    <row r="17" spans="5:13">
+        <v>42.547264352331837</v>
+      </c>
+    </row>
+    <row r="17" spans="5:15">
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="19" spans="5:13">
-      <c r="M19" s="2"/>
-    </row>
-    <row r="20" spans="5:13">
+    <row r="18" spans="5:15">
+      <c r="L18" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+    </row>
+    <row r="19" spans="5:15">
+      <c r="L19" s="20">
+        <v>0.23330000000000001</v>
+      </c>
+      <c r="M19" s="21"/>
+      <c r="N19" s="19"/>
+    </row>
+    <row r="20" spans="5:15">
       <c r="E20" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-    </row>
-    <row r="22" spans="5:13">
+      <c r="L20" s="19"/>
+      <c r="M20" s="22"/>
+      <c r="N20" s="19"/>
+    </row>
+    <row r="21" spans="5:15">
+      <c r="L21" s="7">
+        <f>F11*(1-L19)</f>
+        <v>0.10887139999999998</v>
+      </c>
+      <c r="M21" s="18">
+        <f>F11*L19</f>
+        <v>3.3128600000000001E-2</v>
+      </c>
+      <c r="O21" s="7"/>
+    </row>
+    <row r="22" spans="5:15">
       <c r="H22" s="5"/>
-    </row>
-    <row r="23" spans="5:13">
+      <c r="L22">
+        <f>L21/F8</f>
+        <v>2.150442673509417E-2</v>
+      </c>
+      <c r="M22" s="6">
+        <f>M21/F7</f>
+        <v>6.5365847533632275E-3</v>
+      </c>
+      <c r="N22" s="9">
+        <f>L22+M22</f>
+        <v>2.8041011488457397E-2</v>
+      </c>
+      <c r="O22" s="7"/>
+    </row>
+    <row r="23" spans="5:15">
       <c r="H23" s="5"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="F7:H7">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1563,11 +1835,11 @@
         <v>22</v>
       </c>
       <c r="B7">
-        <f>B5*B6</f>
+        <f t="shared" ref="B7:G7" si="0">B5*B6</f>
         <v>37240</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:G7" si="0">C5*C6</f>
+        <f t="shared" si="0"/>
         <v>27700</v>
       </c>
       <c r="D7">
@@ -1633,10 +1905,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H24"/>
+  <dimension ref="A2:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1645,7 +1917,7 @@
     <col min="4" max="4" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:12">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -1653,46 +1925,50 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:12">
       <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D3" s="1">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="G4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:12">
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="2">
         <f>VLOOKUP(D3,Manager!C11:J16,8,FALSE)</f>
-        <v>58.996078654487874</v>
+        <v>42.547264352331837</v>
       </c>
       <c r="G5" s="14">
         <f>D5/$D$11</f>
-        <v>0.67144563843615479</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>0.58673573024400039</v>
+      </c>
+      <c r="L5">
+        <f>58.7+36.5+2.2+1.6+1</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="C6" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="2">
         <f>VLOOKUP(D3,PE!C11:J16,8,FALSE)</f>
-        <v>24.647657119500725</v>
+        <v>26.499193974264216</v>
       </c>
       <c r="G6" s="14">
-        <f t="shared" ref="G6:G9" si="0">D6/$D$11</f>
-        <v>0.28051969296945239</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
+        <f>D6/$D$11</f>
+        <v>0.36542946212980693</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="C7" s="4" t="s">
         <v>12</v>
       </c>
@@ -1704,17 +1980,17 @@
         <v>37</v>
       </c>
       <c r="G7" s="14">
-        <f t="shared" si="0"/>
-        <v>1.8088143816708955E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <f>D7/$D$11</f>
+        <v>2.191680207873703E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="D8" s="2">
         <f>F8*E8*D$3*1000000/1000000000*2*64</f>
-        <v>1.6012415999999998</v>
+        <v>1.1437440000000001</v>
       </c>
       <c r="E8" s="11">
         <v>4.1999999999999996E-6</v>
@@ -1723,17 +1999,21 @@
         <v>4255</v>
       </c>
       <c r="G8" s="14">
-        <f t="shared" si="0"/>
-        <v>1.8224036460103656E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
+        <f>D8/$D$11</f>
+        <v>1.5772470481181834E-2</v>
+      </c>
+      <c r="J8">
+        <f>(D5+D6)/(175*2)</f>
+        <v>0.19727559521884586</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="C9" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D9" s="2">
         <f>F9*E9*D$3*1000000/1000000000*2*64</f>
-        <v>1.02998784</v>
+        <v>0.73570559999999996</v>
       </c>
       <c r="E9" s="11">
         <v>4.1999999999999996E-6</v>
@@ -1742,31 +2022,31 @@
         <v>2737</v>
       </c>
       <c r="G9" s="14">
-        <f t="shared" si="0"/>
-        <v>1.1722488317580189E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
+        <f>D9/$D$11</f>
+        <v>1.014553506627372E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="H10" s="14">
         <f>SUM(G5:G9)</f>
-        <v>0.99999999999999989</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D11" s="2">
         <f>SUM(D5:D9)</f>
-        <v>87.86426670652591</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
+        <v>72.51520941913337</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="C14" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:12">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -1777,7 +2057,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1801,11 +2081,11 @@
         <v>0.67</v>
       </c>
       <c r="C17" s="10">
-        <f t="shared" ref="C17:D24" si="1">2048*64*C$15/1000000*$B17</f>
+        <f t="shared" ref="C17:D24" si="0">2048*64*C$15/1000000*$B17</f>
         <v>43.909120000000001</v>
       </c>
       <c r="D17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>61.472768000000002</v>
       </c>
     </row>
@@ -1817,11 +2097,11 @@
         <v>0.73</v>
       </c>
       <c r="C18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>47.841279999999998</v>
       </c>
       <c r="D18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>66.977791999999994</v>
       </c>
     </row>
@@ -1833,11 +2113,11 @@
         <v>0.78</v>
       </c>
       <c r="C19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>51.118080000000006</v>
       </c>
       <c r="D19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>71.565312000000006</v>
       </c>
     </row>
@@ -1849,11 +2129,11 @@
         <v>0.84</v>
       </c>
       <c r="C20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>55.050240000000002</v>
       </c>
       <c r="D20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>77.070335999999998</v>
       </c>
     </row>
@@ -1865,11 +2145,11 @@
         <v>0.94</v>
       </c>
       <c r="C21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>61.603839999999998</v>
       </c>
       <c r="D21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>86.245375999999993</v>
       </c>
     </row>
@@ -1881,11 +2161,11 @@
         <v>0.82</v>
       </c>
       <c r="C22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>53.739519999999999</v>
       </c>
       <c r="D22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>75.235327999999996</v>
       </c>
     </row>
@@ -1897,11 +2177,11 @@
         <v>0.89</v>
       </c>
       <c r="C23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>58.327040000000004</v>
       </c>
       <c r="D23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>81.657855999999995</v>
       </c>
     </row>
@@ -1913,11 +2193,11 @@
         <v>0.91</v>
       </c>
       <c r="C24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>59.63776</v>
       </c>
       <c r="D24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>83.492863999999997</v>
       </c>
     </row>

</xml_diff>